<commit_message>
Updated model diagnostics and plots
</commit_message>
<xml_diff>
--- a/results/COVID19tests_model_diagnostics.xlsx
+++ b/results/COVID19tests_model_diagnostics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0784726/Dropbox/Data/devtools/covid19test/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E8CB73-EAFF-DD48-A245-169C4BFA899D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A252C6F0-1B55-8140-9FC2-1E1A365AF400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{ABE7DC77-571B-DF43-8387-E1B703F039B0}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{ABE7DC77-571B-DF43-8387-E1B703F039B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>COVID19 Tests</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Mean absolute error</t>
+  </si>
+  <si>
+    <t>ann probably need normalization to work better</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB505F4-AF9C-154A-8079-F98B3A940DDC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,6 +472,9 @@
       <c r="B6">
         <v>0.96</v>
       </c>
+      <c r="C6">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -477,6 +483,9 @@
       <c r="B7">
         <v>0.64</v>
       </c>
+      <c r="C7">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -485,6 +494,9 @@
       <c r="B8">
         <v>0.65</v>
       </c>
+      <c r="C8">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -493,6 +505,9 @@
       <c r="B9">
         <v>0.67</v>
       </c>
+      <c r="C9">
+        <v>1.03</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -501,15 +516,29 @@
       <c r="B10">
         <v>0.63</v>
       </c>
+      <c r="C10">
+        <v>1.01</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>0.86</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>